<commit_message>
Diferentes analisis para los 24 meses
</commit_message>
<xml_diff>
--- a/analisis_consumos/data/encuesta_consumos_oliver_excel.xlsx
+++ b/analisis_consumos/data/encuesta_consumos_oliver_excel.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Boj\Desktop\GitHub-TFM\analisis_consumos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7799925-84C9-407A-919B-F41586092990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E96A48-BCEA-4BB4-ACE3-4ECF12F35CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38880" yWindow="-21600" windowWidth="38640" windowHeight="21120" xr2:uid="{DFB5D92B-FF0E-43B7-BDE9-DF1730575DF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DFB5D92B-FF0E-43B7-BDE9-DF1730575DF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$W$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1132,7 +1148,7 @@
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,7 +1226,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1222,28 +1238,28 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M2" t="s">
         <v>27</v>
@@ -1273,24 +1289,24 @@
         <v>27</v>
       </c>
       <c r="V2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1302,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
@@ -1311,10 +1327,10 @@
         <v>33</v>
       </c>
       <c r="K3">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
@@ -1344,18 +1360,18 @@
         <v>27</v>
       </c>
       <c r="V3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1364,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1373,19 +1389,19 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
         <v>27</v>
@@ -1412,21 +1428,21 @@
         <v>28</v>
       </c>
       <c r="U4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="W4" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1435,16 +1451,16 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
@@ -1453,13 +1469,13 @@
         <v>33</v>
       </c>
       <c r="K5">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
         <v>28</v>
@@ -1489,12 +1505,12 @@
         <v>29</v>
       </c>
       <c r="W5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1506,49 +1522,49 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K6">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
         <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
         <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s">
         <v>28</v>
       </c>
       <c r="Q6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R6" t="s">
         <v>28</v>
       </c>
       <c r="S6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T6" t="s">
         <v>28</v>
@@ -1557,18 +1573,18 @@
         <v>28</v>
       </c>
       <c r="V6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="W6" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1577,25 +1593,25 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K7">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
         <v>27</v>
@@ -1613,7 +1629,7 @@
         <v>28</v>
       </c>
       <c r="Q7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R7" t="s">
         <v>28</v>
@@ -1628,21 +1644,21 @@
         <v>27</v>
       </c>
       <c r="V7" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1657,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
@@ -1666,7 +1682,7 @@
         <v>33</v>
       </c>
       <c r="K8">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
@@ -1702,21 +1718,21 @@
         <v>27</v>
       </c>
       <c r="W8" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1728,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
@@ -1737,10 +1753,10 @@
         <v>33</v>
       </c>
       <c r="K9">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="M9" t="s">
         <v>34</v>
@@ -1770,48 +1786,48 @@
         <v>27</v>
       </c>
       <c r="V9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W9" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
         <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K10">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="L10" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="M10" t="s">
         <v>27</v>
@@ -1844,15 +1860,15 @@
         <v>29</v>
       </c>
       <c r="W10" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1861,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1870,22 +1886,22 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K11">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="L11" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N11" t="s">
         <v>28</v>
@@ -1903,60 +1919,60 @@
         <v>28</v>
       </c>
       <c r="S11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T11" t="s">
         <v>28</v>
       </c>
       <c r="U11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V11" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="W11" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
         <v>54</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K12">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="N12" t="s">
         <v>28</v>
@@ -1974,7 +1990,7 @@
         <v>28</v>
       </c>
       <c r="S12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T12" t="s">
         <v>28</v>
@@ -1983,28 +1999,28 @@
         <v>27</v>
       </c>
       <c r="V12" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="W12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
         <v>0</v>
       </c>
@@ -2012,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="I13" t="s">
         <v>24</v>
@@ -2021,7 +2037,7 @@
         <v>33</v>
       </c>
       <c r="K13">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
@@ -2039,7 +2055,7 @@
         <v>28</v>
       </c>
       <c r="Q13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R13" t="s">
         <v>28</v>
@@ -2054,18 +2070,18 @@
         <v>28</v>
       </c>
       <c r="V13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W13" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2074,25 +2090,25 @@
         <v>0</v>
       </c>
       <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>2</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
       <c r="H14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K14">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="L14" t="s">
         <v>27</v>
@@ -2122,21 +2138,21 @@
         <v>28</v>
       </c>
       <c r="U14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V14" t="s">
         <v>29</v>
       </c>
       <c r="W14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2145,31 +2161,31 @@
         <v>0</v>
       </c>
       <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="J15" t="s">
         <v>33</v>
       </c>
       <c r="K15">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="L15" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="M15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="N15" t="s">
         <v>28</v>
@@ -2187,7 +2203,7 @@
         <v>28</v>
       </c>
       <c r="S15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T15" t="s">
         <v>28</v>
@@ -2196,21 +2212,21 @@
         <v>28</v>
       </c>
       <c r="V15" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="W15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2222,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I16" t="s">
         <v>73</v>
@@ -2270,30 +2286,30 @@
         <v>29</v>
       </c>
       <c r="W16" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" t="s">
         <v>54</v>
@@ -2305,10 +2321,10 @@
         <v>33</v>
       </c>
       <c r="K17">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="L17" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="M17" t="s">
         <v>27</v>
@@ -2323,7 +2339,7 @@
         <v>28</v>
       </c>
       <c r="Q17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R17" t="s">
         <v>28</v>
@@ -2338,28 +2354,28 @@
         <v>28</v>
       </c>
       <c r="V17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W17" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
         <v>0</v>
       </c>
@@ -2367,28 +2383,28 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K18">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L18" t="s">
         <v>27</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N18" t="s">
         <v>28</v>
       </c>
       <c r="O18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P18" t="s">
         <v>28</v>
@@ -2400,57 +2416,57 @@
         <v>28</v>
       </c>
       <c r="S18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T18" t="s">
         <v>28</v>
       </c>
       <c r="U18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V18" t="s">
         <v>49</v>
       </c>
       <c r="W18" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="G19">
         <v>2</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
       </c>
       <c r="H19" t="s">
         <v>54</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="J19" t="s">
         <v>33</v>
       </c>
       <c r="K19">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="L19" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M19" t="s">
         <v>27</v>
@@ -2471,7 +2487,7 @@
         <v>28</v>
       </c>
       <c r="S19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T19" t="s">
         <v>28</v>
@@ -2480,13 +2496,18 @@
         <v>27</v>
       </c>
       <c r="V19" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="W19" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W1" xr:uid="{4D048549-7C5D-401D-B4AF-FED95174305F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W19">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>